<commit_message>
added most/a likely place to cho-creation-events (cho-event tab are cho's of nl journey) in duerer data
</commit_message>
<xml_diff>
--- a/public/data/data-duerer.xlsx
+++ b/public/data/data-duerer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\duk\InTaVia2023\data-import\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3A3687-19C2-4219-807B-280E50EFFFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC13F50-61E2-4CDB-9B26-9B6AB61D04ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" firstSheet="1" activeTab="9" xr2:uid="{C25329CA-05B7-420C-A3AD-7BFC7999E524}"/>
+    <workbookView xWindow="74865" yWindow="4110" windowWidth="8535" windowHeight="5010" firstSheet="5" activeTab="6" xr2:uid="{C25329CA-05B7-420C-A3AD-7BFC7999E524}"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3713" uniqueCount="1384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3799" uniqueCount="1386">
   <si>
     <t>id</t>
   </si>
@@ -4195,13 +4195,19 @@
   </si>
   <si>
     <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>https://barber.org.uk/wp-content/uploads/2018/06/54.9-Durer500.jpg</t>
+  </si>
+  <si>
+    <t>https://barber.org.uk/albrecht-durer-1471-1528-2/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4264,6 +4270,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -4288,10 +4302,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4356,8 +4371,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4944,7 +4961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F870BEB-B6B1-493D-AF20-4CA3C7300BD9}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -4984,8 +5001,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -5241,7 +5258,9 @@
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="G14" s="3" t="s">
+        <v>1382</v>
+      </c>
       <c r="H14" s="8" t="s">
         <v>638</v>
       </c>
@@ -6802,7 +6821,7 @@
   <dimension ref="A1:J144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I131" sqref="I131"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -9293,8 +9312,8 @@
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="8.9375" style="3"/>
-    <col min="2" max="2" width="13.29296875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.1171875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="28" style="3" customWidth="1"/>
+    <col min="3" max="3" width="60" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.52734375" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.76171875" style="3" customWidth="1"/>
     <col min="6" max="16384" width="8.9375" style="3"/>
@@ -9321,8 +9340,20 @@
       <c r="A2" s="3" t="s">
         <v>1382</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>1384</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>186</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{6555C001-AF61-499A-ABE7-287E901E3F73}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9332,8 +9363,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:N241"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -9348,7 +9379,7 @@
     <col min="8" max="9" width="9.9375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.05859375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.41015625" customWidth="1"/>
-    <col min="12" max="12" width="5.05859375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.46875" customWidth="1"/>
     <col min="13" max="13" width="18.05859375" customWidth="1"/>
     <col min="14" max="14" width="14.05859375" customWidth="1"/>
   </cols>
@@ -9419,7 +9450,9 @@
       <c r="I2" s="8"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
-      <c r="L2" s="8"/>
+      <c r="L2" s="8" t="s">
+        <v>305</v>
+      </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
@@ -9471,8 +9504,12 @@
         <v>15</v>
       </c>
       <c r="K5" s="7"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="L5" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>767</v>
+      </c>
       <c r="N5" s="8"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.5">
@@ -9523,7 +9560,9 @@
         <v>300</v>
       </c>
       <c r="K8" s="7"/>
-      <c r="L8" s="8"/>
+      <c r="L8" t="s">
+        <v>208</v>
+      </c>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
     </row>
@@ -9575,7 +9614,9 @@
         <v>30</v>
       </c>
       <c r="K11" s="7"/>
-      <c r="L11" s="8"/>
+      <c r="L11" t="s">
+        <v>208</v>
+      </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
     </row>
@@ -9627,7 +9668,9 @@
         <v>90</v>
       </c>
       <c r="K14" s="7"/>
-      <c r="L14" s="8"/>
+      <c r="L14" t="s">
+        <v>208</v>
+      </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
     </row>
@@ -9679,7 +9722,9 @@
         <v>90</v>
       </c>
       <c r="K17" s="7"/>
-      <c r="L17" s="8"/>
+      <c r="L17" t="s">
+        <v>208</v>
+      </c>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
     </row>
@@ -9731,7 +9776,9 @@
         <v>10</v>
       </c>
       <c r="K20" s="7"/>
-      <c r="L20" s="8"/>
+      <c r="L20" s="8" t="s">
+        <v>209</v>
+      </c>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
     </row>
@@ -9783,7 +9830,9 @@
         <v>8</v>
       </c>
       <c r="K23" s="7"/>
-      <c r="L23" s="8"/>
+      <c r="L23" s="8" t="s">
+        <v>210</v>
+      </c>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
     </row>
@@ -9837,7 +9886,9 @@
       <c r="K26" s="23" t="s">
         <v>886</v>
       </c>
-      <c r="L26" s="8"/>
+      <c r="L26" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M26" s="8"/>
       <c r="N26" s="8"/>
     </row>
@@ -9889,7 +9940,9 @@
         <v>15</v>
       </c>
       <c r="K29" s="7"/>
-      <c r="L29" s="8"/>
+      <c r="L29" t="s">
+        <v>207</v>
+      </c>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
     </row>
@@ -9941,7 +9994,9 @@
         <v>10</v>
       </c>
       <c r="K32" s="7"/>
-      <c r="L32" s="8"/>
+      <c r="L32" t="s">
+        <v>207</v>
+      </c>
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
     </row>
@@ -9993,7 +10048,9 @@
         <v>10</v>
       </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="8"/>
+      <c r="L35" t="s">
+        <v>207</v>
+      </c>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
     </row>
@@ -10045,7 +10102,9 @@
         <v>10</v>
       </c>
       <c r="K38" s="7"/>
-      <c r="L38" s="8"/>
+      <c r="L38" t="s">
+        <v>207</v>
+      </c>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
     </row>
@@ -10097,7 +10156,9 @@
         <v>3</v>
       </c>
       <c r="K41" s="7"/>
-      <c r="L41" s="8"/>
+      <c r="L41" t="s">
+        <v>414</v>
+      </c>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
     </row>
@@ -10149,7 +10210,9 @@
         <v>10</v>
       </c>
       <c r="K44" s="7"/>
-      <c r="L44" s="8"/>
+      <c r="L44" t="s">
+        <v>207</v>
+      </c>
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
     </row>
@@ -10201,7 +10264,9 @@
         <v>14</v>
       </c>
       <c r="K47" s="7"/>
-      <c r="L47" s="8"/>
+      <c r="L47" t="s">
+        <v>206</v>
+      </c>
       <c r="M47" s="8"/>
       <c r="N47" s="8"/>
     </row>
@@ -10253,7 +10318,9 @@
         <v>5</v>
       </c>
       <c r="K50" s="7"/>
-      <c r="L50" s="8"/>
+      <c r="L50" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="M50" s="8"/>
       <c r="N50" s="8"/>
     </row>
@@ -10305,7 +10372,9 @@
         <v>10</v>
       </c>
       <c r="K53" s="7"/>
-      <c r="L53" s="8"/>
+      <c r="L53" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M53" s="8"/>
       <c r="N53" s="8"/>
     </row>
@@ -10357,7 +10426,9 @@
         <v>4</v>
       </c>
       <c r="K56" s="7"/>
-      <c r="L56" s="8"/>
+      <c r="L56" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M56" s="8"/>
       <c r="N56" s="8"/>
     </row>
@@ -10409,7 +10480,9 @@
         <v>180</v>
       </c>
       <c r="K59" s="7"/>
-      <c r="L59" s="8"/>
+      <c r="L59" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M59" s="8"/>
       <c r="N59" s="8"/>
     </row>
@@ -10461,7 +10534,9 @@
         <v>10</v>
       </c>
       <c r="K62" s="7"/>
-      <c r="L62" s="8"/>
+      <c r="L62" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M62" s="8"/>
       <c r="N62" s="8"/>
     </row>
@@ -10513,7 +10588,9 @@
         <v>300</v>
       </c>
       <c r="K65" s="7"/>
-      <c r="L65" s="8"/>
+      <c r="L65" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M65" s="8"/>
       <c r="N65" s="8"/>
     </row>
@@ -10565,7 +10642,9 @@
         <v>300</v>
       </c>
       <c r="K68" s="7"/>
-      <c r="L68" s="8"/>
+      <c r="L68" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M68" s="8"/>
       <c r="N68" s="8"/>
     </row>
@@ -10617,7 +10696,9 @@
         <v>300</v>
       </c>
       <c r="K71" s="7"/>
-      <c r="L71" s="8"/>
+      <c r="L71" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M71" s="8"/>
       <c r="N71" s="8"/>
     </row>
@@ -10669,7 +10750,9 @@
         <v>250</v>
       </c>
       <c r="K74" s="7"/>
-      <c r="L74" s="8"/>
+      <c r="L74" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M74" s="8"/>
       <c r="N74" s="8"/>
     </row>
@@ -10721,7 +10804,9 @@
         <v>250</v>
       </c>
       <c r="K77" s="7"/>
-      <c r="L77" s="8"/>
+      <c r="L77" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M77" s="8"/>
       <c r="N77" s="8"/>
     </row>
@@ -10773,7 +10858,9 @@
         <v>300</v>
       </c>
       <c r="K80" s="7"/>
-      <c r="L80" s="8"/>
+      <c r="L80" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M80" s="8"/>
       <c r="N80" s="8"/>
     </row>
@@ -10825,7 +10912,9 @@
         <v>300</v>
       </c>
       <c r="K83" s="7"/>
-      <c r="L83" s="8"/>
+      <c r="L83" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M83" s="8"/>
       <c r="N83" s="8"/>
     </row>
@@ -10877,7 +10966,9 @@
         <v>15</v>
       </c>
       <c r="K86" s="7"/>
-      <c r="L86" s="8"/>
+      <c r="L86" t="s">
+        <v>207</v>
+      </c>
       <c r="M86" s="8"/>
       <c r="N86" s="8"/>
     </row>
@@ -10929,7 +11020,9 @@
         <v>90</v>
       </c>
       <c r="K89" s="7"/>
-      <c r="L89" s="8"/>
+      <c r="L89" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M89" s="8"/>
       <c r="N89" s="8"/>
     </row>
@@ -10981,7 +11074,9 @@
         <v>90</v>
       </c>
       <c r="K92" s="7"/>
-      <c r="L92" s="8"/>
+      <c r="L92" t="s">
+        <v>208</v>
+      </c>
       <c r="M92" s="8"/>
       <c r="N92" s="8"/>
     </row>
@@ -11033,7 +11128,9 @@
         <v>300</v>
       </c>
       <c r="K95" s="7"/>
-      <c r="L95" s="8"/>
+      <c r="L95" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M95" s="8"/>
       <c r="N95" s="8"/>
     </row>
@@ -11085,7 +11182,9 @@
         <v>90</v>
       </c>
       <c r="K98" s="7"/>
-      <c r="L98" s="8"/>
+      <c r="L98" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M98" s="8"/>
       <c r="N98" s="8"/>
     </row>
@@ -11137,7 +11236,9 @@
         <v>300</v>
       </c>
       <c r="K101" s="7"/>
-      <c r="L101" s="8"/>
+      <c r="L101" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M101" s="8"/>
       <c r="N101" s="8"/>
     </row>
@@ -11189,7 +11290,9 @@
         <v>300</v>
       </c>
       <c r="K104" s="7"/>
-      <c r="L104" s="8"/>
+      <c r="L104" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M104" s="8"/>
       <c r="N104" s="8"/>
     </row>
@@ -11239,7 +11342,9 @@
       <c r="I107" s="8"/>
       <c r="J107" s="7"/>
       <c r="K107" s="7"/>
-      <c r="L107" s="8"/>
+      <c r="L107" s="8" t="s">
+        <v>212</v>
+      </c>
       <c r="M107" s="8"/>
       <c r="N107" s="8"/>
     </row>
@@ -11289,7 +11394,9 @@
       <c r="I110" s="8"/>
       <c r="J110" s="7"/>
       <c r="K110" s="7"/>
-      <c r="L110" s="8"/>
+      <c r="L110" s="8" t="s">
+        <v>212</v>
+      </c>
       <c r="M110" s="8"/>
       <c r="N110" s="8"/>
     </row>
@@ -11341,7 +11448,9 @@
         <v>2</v>
       </c>
       <c r="K113" s="7"/>
-      <c r="L113" s="8"/>
+      <c r="L113" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="M113" s="8"/>
       <c r="N113" s="8"/>
     </row>
@@ -11393,7 +11502,9 @@
         <v>300</v>
       </c>
       <c r="K116" s="7"/>
-      <c r="L116" s="8"/>
+      <c r="L116" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="M116" s="8"/>
       <c r="N116" s="8"/>
     </row>
@@ -11445,7 +11556,9 @@
         <v>8</v>
       </c>
       <c r="K119" s="7"/>
-      <c r="L119" s="8"/>
+      <c r="L119" s="8" t="s">
+        <v>434</v>
+      </c>
       <c r="M119" s="8"/>
       <c r="N119" s="8"/>
     </row>
@@ -11497,7 +11610,9 @@
         <v>120</v>
       </c>
       <c r="K122" s="7"/>
-      <c r="L122" s="8"/>
+      <c r="L122" t="s">
+        <v>208</v>
+      </c>
       <c r="M122" s="8"/>
       <c r="N122" s="8"/>
     </row>
@@ -11549,7 +11664,9 @@
         <v>120</v>
       </c>
       <c r="K125" s="7"/>
-      <c r="L125" s="8"/>
+      <c r="L125" t="s">
+        <v>208</v>
+      </c>
       <c r="M125" s="8"/>
       <c r="N125" s="8"/>
     </row>
@@ -11601,7 +11718,9 @@
         <v>1</v>
       </c>
       <c r="K128" s="7"/>
-      <c r="L128" s="8"/>
+      <c r="L128" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="M128" s="8"/>
       <c r="N128" s="8"/>
     </row>
@@ -11653,7 +11772,9 @@
         <v>15</v>
       </c>
       <c r="K131" s="7"/>
-      <c r="L131" s="8"/>
+      <c r="L131" t="s">
+        <v>208</v>
+      </c>
       <c r="M131" s="8"/>
       <c r="N131" s="8"/>
     </row>
@@ -11705,7 +11826,9 @@
         <v>30</v>
       </c>
       <c r="K134" s="7"/>
-      <c r="L134" s="8"/>
+      <c r="L134" t="s">
+        <v>208</v>
+      </c>
       <c r="M134" s="8"/>
       <c r="N134" s="8"/>
     </row>
@@ -11757,7 +11880,9 @@
         <v>30</v>
       </c>
       <c r="K137" s="7"/>
-      <c r="L137" s="8"/>
+      <c r="L137" t="s">
+        <v>208</v>
+      </c>
       <c r="M137" s="8"/>
       <c r="N137" s="8"/>
     </row>
@@ -11809,7 +11934,9 @@
         <v>30</v>
       </c>
       <c r="K140" s="7"/>
-      <c r="L140" s="8"/>
+      <c r="L140" t="s">
+        <v>208</v>
+      </c>
       <c r="M140" s="8"/>
       <c r="N140" s="8"/>
     </row>
@@ -11861,7 +11988,9 @@
         <v>25</v>
       </c>
       <c r="K143" s="7"/>
-      <c r="L143" s="8"/>
+      <c r="L143" t="s">
+        <v>208</v>
+      </c>
       <c r="M143" s="8"/>
       <c r="N143" s="8"/>
     </row>
@@ -11913,7 +12042,9 @@
         <v>25</v>
       </c>
       <c r="K146" s="7"/>
-      <c r="L146" s="8"/>
+      <c r="L146" t="s">
+        <v>208</v>
+      </c>
       <c r="M146" s="8"/>
       <c r="N146" s="8"/>
     </row>
@@ -11965,7 +12096,9 @@
         <v>25</v>
       </c>
       <c r="K149" s="7"/>
-      <c r="L149" s="8"/>
+      <c r="L149" t="s">
+        <v>208</v>
+      </c>
       <c r="M149" s="8"/>
       <c r="N149" s="8"/>
     </row>
@@ -12017,7 +12150,9 @@
         <v>120</v>
       </c>
       <c r="K152" s="7"/>
-      <c r="L152" s="8"/>
+      <c r="L152" t="s">
+        <v>208</v>
+      </c>
       <c r="M152" s="8"/>
       <c r="N152" s="8"/>
     </row>
@@ -12069,7 +12204,9 @@
         <v>25</v>
       </c>
       <c r="K155" s="7"/>
-      <c r="L155" s="8"/>
+      <c r="L155" t="s">
+        <v>208</v>
+      </c>
       <c r="M155" s="8"/>
       <c r="N155" s="8"/>
     </row>
@@ -12121,7 +12258,9 @@
         <v>300</v>
       </c>
       <c r="K158" s="7"/>
-      <c r="L158" s="8"/>
+      <c r="L158" t="s">
+        <v>208</v>
+      </c>
       <c r="M158" s="8"/>
       <c r="N158" s="8"/>
     </row>
@@ -12173,7 +12312,9 @@
         <v>6</v>
       </c>
       <c r="K161" s="7"/>
-      <c r="L161" s="8"/>
+      <c r="L161" t="s">
+        <v>210</v>
+      </c>
       <c r="M161" s="8"/>
       <c r="N161" s="8"/>
     </row>
@@ -12225,7 +12366,9 @@
         <v>120</v>
       </c>
       <c r="K164" s="7"/>
-      <c r="L164" s="8"/>
+      <c r="L164" t="s">
+        <v>208</v>
+      </c>
       <c r="M164" s="8"/>
       <c r="N164" s="8"/>
     </row>
@@ -12277,7 +12420,9 @@
         <v>210</v>
       </c>
       <c r="K167" s="7"/>
-      <c r="L167" s="8"/>
+      <c r="L167" t="s">
+        <v>208</v>
+      </c>
       <c r="M167" s="8"/>
       <c r="N167" s="8"/>
     </row>
@@ -12329,7 +12474,9 @@
         <v>300</v>
       </c>
       <c r="K170" s="7"/>
-      <c r="L170" s="8"/>
+      <c r="L170" t="s">
+        <v>208</v>
+      </c>
       <c r="M170" s="8"/>
       <c r="N170" s="8"/>
     </row>
@@ -12381,7 +12528,9 @@
         <v>210</v>
       </c>
       <c r="K173" s="7"/>
-      <c r="L173" s="8"/>
+      <c r="L173" t="s">
+        <v>208</v>
+      </c>
       <c r="M173" s="8"/>
       <c r="N173" s="8"/>
     </row>
@@ -12433,7 +12582,9 @@
         <v>210</v>
       </c>
       <c r="K176" s="7"/>
-      <c r="L176" s="8"/>
+      <c r="L176" t="s">
+        <v>208</v>
+      </c>
       <c r="M176" s="8"/>
       <c r="N176" s="8"/>
     </row>
@@ -12485,7 +12636,9 @@
         <v>210</v>
       </c>
       <c r="K179" s="7"/>
-      <c r="L179" s="8"/>
+      <c r="L179" t="s">
+        <v>208</v>
+      </c>
       <c r="M179" s="8"/>
       <c r="N179" s="8"/>
     </row>
@@ -12537,7 +12690,9 @@
         <v>300</v>
       </c>
       <c r="K182" s="7"/>
-      <c r="L182" s="8"/>
+      <c r="L182" t="s">
+        <v>208</v>
+      </c>
       <c r="M182" s="8"/>
       <c r="N182" s="8"/>
     </row>
@@ -12589,7 +12744,9 @@
         <v>15</v>
       </c>
       <c r="K185" s="7"/>
-      <c r="L185" s="8"/>
+      <c r="L185" t="s">
+        <v>208</v>
+      </c>
       <c r="M185" s="8"/>
       <c r="N185" s="8"/>
     </row>
@@ -12641,7 +12798,9 @@
         <v>60</v>
       </c>
       <c r="K188" s="7"/>
-      <c r="L188" s="8"/>
+      <c r="L188" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M188" s="8"/>
       <c r="N188" s="8"/>
     </row>
@@ -12691,7 +12850,9 @@
       <c r="I191" s="8"/>
       <c r="J191" s="7"/>
       <c r="K191" s="7"/>
-      <c r="L191" s="8"/>
+      <c r="L191" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M191" s="8"/>
       <c r="N191" s="8"/>
     </row>
@@ -12743,7 +12904,9 @@
         <v>4</v>
       </c>
       <c r="K194" s="7"/>
-      <c r="L194" s="8"/>
+      <c r="L194" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M194" s="8"/>
       <c r="N194" s="8"/>
     </row>
@@ -12795,7 +12958,9 @@
         <v>300</v>
       </c>
       <c r="K197" s="7"/>
-      <c r="L197" s="8"/>
+      <c r="L197" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M197" s="8"/>
       <c r="N197" s="8"/>
     </row>
@@ -12847,7 +13012,9 @@
         <v>15</v>
       </c>
       <c r="K200" s="7"/>
-      <c r="L200" s="8"/>
+      <c r="L200" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M200" s="8"/>
       <c r="N200" s="8"/>
     </row>
@@ -12899,7 +13066,9 @@
         <v>60</v>
       </c>
       <c r="K203" s="7"/>
-      <c r="L203" s="8"/>
+      <c r="L203" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M203" s="8"/>
       <c r="N203" s="8"/>
     </row>
@@ -12951,7 +13120,9 @@
         <v>210</v>
       </c>
       <c r="K206" s="7"/>
-      <c r="L206" s="8"/>
+      <c r="L206" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M206" s="8"/>
       <c r="N206" s="8"/>
     </row>
@@ -13003,7 +13174,9 @@
         <v>120</v>
       </c>
       <c r="K209" s="7"/>
-      <c r="L209" s="8"/>
+      <c r="L209" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M209" s="8"/>
       <c r="N209" s="8"/>
     </row>
@@ -13055,7 +13228,9 @@
         <v>3</v>
       </c>
       <c r="K212" s="7"/>
-      <c r="L212" s="8"/>
+      <c r="L212" s="8" t="s">
+        <v>210</v>
+      </c>
       <c r="M212" s="8"/>
       <c r="N212" s="8"/>
     </row>
@@ -13107,7 +13282,9 @@
         <v>210</v>
       </c>
       <c r="K215" s="7"/>
-      <c r="L215" s="8"/>
+      <c r="L215" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="M215" s="8"/>
       <c r="N215" s="8"/>
     </row>
@@ -13159,7 +13336,9 @@
         <v>60</v>
       </c>
       <c r="K218" s="7"/>
-      <c r="L218" s="8"/>
+      <c r="L218" t="s">
+        <v>208</v>
+      </c>
       <c r="M218" s="8"/>
       <c r="N218" s="8"/>
     </row>
@@ -13211,7 +13390,9 @@
         <v>180</v>
       </c>
       <c r="K221" s="7"/>
-      <c r="L221" s="8"/>
+      <c r="L221" t="s">
+        <v>208</v>
+      </c>
       <c r="M221" s="8"/>
       <c r="N221" s="8"/>
     </row>
@@ -13263,7 +13444,9 @@
         <v>180</v>
       </c>
       <c r="K224" s="7"/>
-      <c r="L224" s="8"/>
+      <c r="L224" t="s">
+        <v>208</v>
+      </c>
       <c r="M224" s="8"/>
       <c r="N224" s="8"/>
     </row>
@@ -13315,7 +13498,9 @@
         <v>180</v>
       </c>
       <c r="K227" s="7"/>
-      <c r="L227" s="8"/>
+      <c r="L227" t="s">
+        <v>208</v>
+      </c>
       <c r="M227" s="8"/>
       <c r="N227" s="8"/>
     </row>
@@ -13367,7 +13552,9 @@
         <v>180</v>
       </c>
       <c r="K230" s="7"/>
-      <c r="L230" s="8"/>
+      <c r="L230" t="s">
+        <v>208</v>
+      </c>
       <c r="M230" s="8"/>
       <c r="N230" s="8"/>
     </row>
@@ -13419,7 +13606,9 @@
         <v>300</v>
       </c>
       <c r="K233" s="7"/>
-      <c r="L233" s="8"/>
+      <c r="L233" t="s">
+        <v>208</v>
+      </c>
       <c r="M233" s="8"/>
       <c r="N233" s="8"/>
     </row>
@@ -13471,7 +13660,9 @@
         <v>210</v>
       </c>
       <c r="K236" s="7"/>
-      <c r="L236" s="8"/>
+      <c r="L236" t="s">
+        <v>208</v>
+      </c>
       <c r="M236" s="8"/>
       <c r="N236" s="8"/>
     </row>
@@ -13523,7 +13714,9 @@
         <v>5</v>
       </c>
       <c r="K239" s="7"/>
-      <c r="L239" s="8"/>
+      <c r="L239" t="s">
+        <v>208</v>
+      </c>
       <c r="M239" s="8"/>
       <c r="N239" s="8"/>
     </row>
@@ -13560,8 +13753,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -15502,8 +15695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DE7CD6-3992-47BC-A701-56D724BB2518}">
   <dimension ref="A1:N169"/>
   <sheetViews>
-    <sheetView topLeftCell="C72" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="E118" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127:XFD127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -19046,6 +19239,9 @@
       <c r="G127" t="s">
         <v>124</v>
       </c>
+      <c r="H127" t="s">
+        <v>753</v>
+      </c>
       <c r="K127" t="s">
         <v>825</v>
       </c>

</xml_diff>

<commit_message>
added media resources and biographies to duerer data
</commit_message>
<xml_diff>
--- a/public/data/data-duerer.xlsx
+++ b/public/data/data-duerer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\duk\InTaVia2023\data-import\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC13F50-61E2-4CDB-9B26-9B6AB61D04ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFC628D-7D5A-4CD7-A34B-DF1CA718B97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="74865" yWindow="4110" windowWidth="8535" windowHeight="5010" firstSheet="5" activeTab="6" xr2:uid="{C25329CA-05B7-420C-A3AD-7BFC7999E524}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" xr2:uid="{C25329CA-05B7-420C-A3AD-7BFC7999E524}"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3799" uniqueCount="1386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4119" uniqueCount="1580">
   <si>
     <t>id</t>
   </si>
@@ -4185,29 +4185,614 @@
     <t>unplanned stay due to error of coachman, overnight stay, probably Aldenhoven</t>
   </si>
   <si>
-    <t>html</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Donec purus urna, vestibulum at purus eget, ultricies commodo justo. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia curae; Donec ullamcorper sapien at massa convallis, a scelerisque orci pretium. Quisque scelerisque iaculis condimentum. Morbi euismod dui et dignissim vulputate. Vestibulum ut ex in est malesuada finibus sed non risus. Aenean eget lobortis lacus, in vehicula purus.</t>
-  </si>
-  <si>
     <t>m-001</t>
   </si>
   <si>
     <t xml:space="preserve">    </t>
   </si>
   <si>
-    <t>https://barber.org.uk/wp-content/uploads/2018/06/54.9-Durer500.jpg</t>
-  </si>
-  <si>
     <t>https://barber.org.uk/albrecht-durer-1471-1528-2/</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>gnd:118924710</t>
+  </si>
+  <si>
+    <t>gnd:118560093</t>
+  </si>
+  <si>
+    <t>gnd:11852786X</t>
+  </si>
+  <si>
+    <t>gnd:118869051</t>
+  </si>
+  <si>
+    <t>gnd:12231297X</t>
+  </si>
+  <si>
+    <t>gnd:119195380</t>
+  </si>
+  <si>
+    <t>wiki:Q1990389</t>
+  </si>
+  <si>
+    <t>gnd:118771175</t>
+  </si>
+  <si>
+    <t>gnd:118563890</t>
+  </si>
+  <si>
+    <t>gnd:118610430</t>
+  </si>
+  <si>
+    <t>https://uploads2.wikiart.org/images/albrecht-durer/portrait-of-lazarus-ravensburger-and-the-turrets-of-the-court-of-lier-in-antwerp.jpg</t>
+  </si>
+  <si>
+    <t>https://www.wikiart.org/en/albrecht-durer/portrait-of-lazarus-ravensburger-and-the-turrets-of-the-court-of-lier-in-antwerp</t>
+  </si>
+  <si>
+    <t>m-002</t>
+  </si>
+  <si>
+    <t>Portrait of Lazarus Ravensburger and the turrets of the court of Lier in Antwerp</t>
+  </si>
+  <si>
+    <t>A Man with an Oar</t>
+  </si>
+  <si>
+    <t>https://barber.org.uk/wp-content/uploads/2018/06/54.9-Durer1200.jpg</t>
+  </si>
+  <si>
+    <t>m-003</t>
+  </si>
+  <si>
+    <t>Portrait of Jobst Plankfelt</t>
+  </si>
+  <si>
+    <t>http://sammlungenonline.albertina.at/cc/imageproxy.ashx?server=localhost&amp;port=15001&amp;filename=images/3162.JPG</t>
+  </si>
+  <si>
+    <t>m-004</t>
+  </si>
+  <si>
+    <t>Portrait of Felix Hungersperg</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/?query=search=/record/objectnumbersearch=[3162]&amp;showtype=record</t>
+  </si>
+  <si>
+    <t>https://staedelmuseum.de/go/ds/699z</t>
+  </si>
+  <si>
+    <t>bio-001</t>
+  </si>
+  <si>
+    <t>biographies</t>
+  </si>
+  <si>
+    <t>bio-002</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Albrecht_D%C3%Bcrer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Albrecht Dürer (21 May 1471 – 6 April 1528) [...] was a German painter, printmaker, and theorist of the German Renaissance. Born in Nuremberg, Dürer established his reputation and influence across Europe in his twenties due to his high-quality woodcut prints. He was in contact with the major Italian artists of his time, including Raphael, Giovanni Bellini, and Leonardo da Vinci, and from 1512 was patronized by Emperor Maximilian I.
+Dürer's vast body of work includes engravings, his preferred technique in his later prints, altarpieces, portraits and self-portraits, watercolours and books. The woodcuts series are more Gothic than the rest of his work. His well-known engravings include the three Meisterstiche (master prints) Knight, Death and the Devil (1513), Saint Jerome in his Study (1514), and Melencolia I (1514). His watercolours mark him as one of the first European landscape artists, while his woodcuts revolutionised the potential of that medium.
+Dürer's introduction of classical motifs into Northern art, through his knowledge of Italian artists and German humanists, has secured his reputation as one of the most important figures of the Northern Renaissance. This is reinforced by his theoretical treatises, which involve principles of mathematics, perspective, and ideal proportions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agnes Dürer née Frey (1475–1539) was the wife of the German artist Albrecht Dürer. During their marriage, which was childless, she was portrayed several times by Dürer.
+Agnes Dürer was the daughter of the coppersmith and lute maker Hans Frey and his wife Anna, a member of the patrician family Rummel. </t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Agnes_D%C3%Bcrer</t>
+  </si>
+  <si>
+    <t>m-005</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/0/02/Agnes_Duerer_1521.jpg</t>
+  </si>
+  <si>
+    <t>Agnes Dürer in traditional Dutch costume</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/File:Agnes_Duerer_1521.jpg</t>
+  </si>
+  <si>
+    <t>"Agnes Dürerin in niederländischer Tracht", Metallstiftzeichnung von Albrecht Dürer.</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Albrecht_D%C3%BCrer_-_1500_self-portrait_(High_resolution_and_detail).jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/d/dc/Albrecht_D%C3%BCrer_-_1500_self-portrait_%28High_resolution_and_detail%29.jpg</t>
+  </si>
+  <si>
+    <t>m-006</t>
+  </si>
+  <si>
+    <t>m-017</t>
+  </si>
+  <si>
+    <t>m-008</t>
+  </si>
+  <si>
+    <t>m-007</t>
+  </si>
+  <si>
+    <t>m-009</t>
+  </si>
+  <si>
+    <t>m-010</t>
+  </si>
+  <si>
+    <t>m-011</t>
+  </si>
+  <si>
+    <t>m-012</t>
+  </si>
+  <si>
+    <t>m-013</t>
+  </si>
+  <si>
+    <t>m-014</t>
+  </si>
+  <si>
+    <t>m-015</t>
+  </si>
+  <si>
+    <t>m-016</t>
+  </si>
+  <si>
+    <t>m-018</t>
+  </si>
+  <si>
+    <t>m-019</t>
+  </si>
+  <si>
+    <t>m-020</t>
+  </si>
+  <si>
+    <t>m-021</t>
+  </si>
+  <si>
+    <t>m-022</t>
+  </si>
+  <si>
+    <t>m-023</t>
+  </si>
+  <si>
+    <t>https://www.bildindex.de/media/large/mi/03/97/6a/mi03976a05.jpg?Expires=1677759882&amp;Signature=hWeVgz5cjlYCBB2LCiBgpEX8KcG3RfTFq0uPL84nDEqrdHhy5ubRwrJVjKuEWzf92X13ypwWFMGToksoUmCw2HPJSF~1JI8zBmob43tSWRXG7P0H5U3DKehqf2tfXUma7o~ZU42ct2Rf9FcwuOsC6EEw2QvAlzU7pO6W7wfrA18_&amp;Key-Pair-Id=APKAJGHHKKX2FHRP63AQ</t>
+  </si>
+  <si>
+    <t>https://www.bildindex.de/document/obj00030696?medium=mi03976a05&amp;part=1</t>
+  </si>
+  <si>
+    <t>Ein Goldschmied aus Mecheln</t>
+  </si>
+  <si>
+    <t>m-024</t>
+  </si>
+  <si>
+    <t>m-025</t>
+  </si>
+  <si>
+    <t>m-026</t>
+  </si>
+  <si>
+    <t>m-027</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/?query=search=/record/objectnumbersearch=[3161]&amp;showtype=record</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/cc/imageproxy.ashx?server=localhost&amp;port=16001&amp;filename=images/3161.JPG</t>
+  </si>
+  <si>
+    <t>https://uploads4.wikiart.org/images/albrecht-durer/portrait-of-paul-martin-and-the-topler-pfinzig.jpg</t>
+  </si>
+  <si>
+    <t>https://www.wikiart.org/en/albrecht-durer/portrait-of-paul-martin-and-the-topler-pfinzig</t>
+  </si>
+  <si>
+    <t>https://www.britishmuseum.org/collection/object/P_1895-0915-982</t>
+  </si>
+  <si>
+    <t>https://media.britishmuseum.org/media/Repository/Documents/2014_11/12_22/3bf094b1_b130_4ca4_b521_a3e1016b5147/large_00136096_001.jpg</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/?query=search=/record/objectnumbersearch=[22385r]&amp;showtype=record</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/cc/imageproxy.ashx?server=localhost&amp;port=16001&amp;filename=images/22385r.JPG</t>
+  </si>
+  <si>
+    <t>A girl from Cologne and Agnes Dürer, near Boppard on the Rhine</t>
+  </si>
+  <si>
+    <t>https://rkd.nl/nl/explore/images/293320</t>
+  </si>
+  <si>
+    <t>https://images.rkd.nl/rkd/thumb/650x650/ba2b4991-b4cd-13b3-32f2-55ff2b82af0e.jpg</t>
+  </si>
+  <si>
+    <t>https://www.brabantserfgoed.nl/image/2019/10/29/585646.jpg</t>
+  </si>
+  <si>
+    <t>Een meisje uit Bergen op Zoom (links) en een meisje uit Goes (rechts), getekend door Albrecht Dürer in 1520. (Bron: Chantilly, musée Condé)</t>
+  </si>
+  <si>
+    <t>https://www.brabantserfgoed.nl/page/10266/twee-gewone-vrouwen-uit-bergen-op-zoom-getekend-door-albrecht-d%C3%BCrer</t>
+  </si>
+  <si>
+    <t>https://sammlung.staedelmuseum.de/en/work/the-new-choir-of-st-gertrudis-in-bergen-op-zoom</t>
+  </si>
+  <si>
+    <t>https://media.britishmuseum.org/media/Repository/Documents/2014_9/29_18/64a81b90_f52e_4794_bc34_a3b501317e9c/mid_00154486_001.jpg</t>
+  </si>
+  <si>
+    <t>https://www.britishmuseum.org/collection/object/P_1921-0714-2</t>
+  </si>
+  <si>
+    <t>https://www.britishmuseum.org/collection/image/154487001</t>
+  </si>
+  <si>
+    <t>https://media.britishmuseum.org/media/Repository/Documents/2014_9/29_18/fb886624_b508_4fe4_8242_a3b50131809f/mid_00154487_001.jpg</t>
+  </si>
+  <si>
+    <t>https://www.britishmuseum.org/collection/image/154436001</t>
+  </si>
+  <si>
+    <t>https://media.britishmuseum.org/media/Repository/Documents/2014_9/29_18/f1ae6fad_e277_4ce7_a508_a3b5013182a7/mid_00154436_001.jpg</t>
+  </si>
+  <si>
+    <t>https://www.britishmuseum.org/collection/object/P_1848-1125-3</t>
+  </si>
+  <si>
+    <t>https://media.britishmuseum.org/media/Repository/Documents/2014_9/29_18/43dbb970_504e_4180_b28a_a3b501317bc2/mid_00154434_001.jpg</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/?query=search=/record/objectnumbersearch=[22385v]&amp;showtype=record</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/cc/imageproxy.ashx?server=localhost&amp;port=16001&amp;filename=images/22385v.JPG</t>
+  </si>
+  <si>
+    <t>Evtl. Burg Rheinfels bei Goslar und Burg Stolzenfels, aus dem Silberstiftskizzenbuch, das während der Reise in die Niederlande entstand</t>
+  </si>
+  <si>
+    <t>http://www.zeno.org/Kunstwerke/B/D%C3%BCrer,%20Albrecht:%20Zwei%20Burgen</t>
+  </si>
+  <si>
+    <t>Two Castles</t>
+  </si>
+  <si>
+    <t>http://images.zeno.org/Kunstwerke/I/big/2540011a.jpg</t>
+  </si>
+  <si>
+    <t>https://sammlung.staedelmuseum.de/en/work/marx-ulstat-the-beautiful-young-woman-of-antwerp</t>
+  </si>
+  <si>
+    <t>Marx Ulstat; The Beautiful Young Woman of Antwerp, ca. 1520 – 1521</t>
+  </si>
+  <si>
+    <t>m-028</t>
+  </si>
+  <si>
+    <t>m-029</t>
+  </si>
+  <si>
+    <t>m-030</t>
+  </si>
+  <si>
+    <t>m-031</t>
+  </si>
+  <si>
+    <t>m-032</t>
+  </si>
+  <si>
+    <t>m-033</t>
+  </si>
+  <si>
+    <t>m-034</t>
+  </si>
+  <si>
+    <t>m-035</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/?query=search=/record/objectnumbersearch=[3167]&amp;showtype=record</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/cc/imageproxy.ashx?server=localhost&amp;port=16001&amp;filename=images/3167.JPG</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/cc/imageproxy.ashx?server=localhost&amp;port=16001&amp;filename=images/3168.JPG</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/?query=search=/record/objectnumbersearch=[3176]&amp;showtype=record</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/cc/imageproxy.ashx?server=localhost&amp;port=16001&amp;filename=images/3176.JPG</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/?query=search=/record/objectnumbersearch=[3175]&amp;showtype=record</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/cc/imageproxy.ashx?server=localhost&amp;port=16001&amp;filename=images/3175.JPG</t>
+  </si>
+  <si>
+    <t>https://sammlung.staedelmuseum.de/en/work/agony-in-the-garden</t>
+  </si>
+  <si>
+    <t>https://proxy.europeana.eu/199/item_THLBWXQUDV5ZKB2ILHXPOOBXMZJMKFOH?view=http%3A%2F%2Fwww.bildindex.de%2Fbilder%2Fd%2Fmi04673b05&amp;disposition=inline&amp;api_url=https%3A%2F%2Fapi.europeana.eu%2Fapi</t>
+  </si>
+  <si>
+    <t>https://www.europeana.eu/de/item/199/item_THLBWXQUDV5ZKB2ILHXPOOBXMZJMKFOH</t>
+  </si>
+  <si>
+    <t>https://www.britishmuseum.org/collection/object/P_1910-0212-103</t>
+  </si>
+  <si>
+    <t>https://media.britishmuseum.org/media/Repository/Documents/2014_9/29_18/1cf4fe6c_5bd4_472e_8060_a3b50131e188/mid_00154525_001.jpg</t>
+  </si>
+  <si>
+    <t>https://www.britishmuseum.org/collection/object/P_SL-5218-48</t>
+  </si>
+  <si>
+    <t>Portrait of Christian II of Denmark</t>
+  </si>
+  <si>
+    <t>https://media.britishmuseum.org/media/Repository/Documents/2014_10/4_14/3d509415_1836_4b7b_8cb5_a3ba00f4062f/mid_00238245_001.jpg</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/cc/imageproxy.ashx?server=localhost&amp;port=16001&amp;filename=images/3163.JPG</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/?query=search=/record/objectnumbersearch=[3163]&amp;showtype=record</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/?query=search=/record/objectnumbersearch=[3165]&amp;showtype=record</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/cc/imageproxy.ashx?server=localhost&amp;port=16001&amp;filename=images/3165.JPG</t>
+  </si>
+  <si>
+    <t>https://www.britishmuseum.org/collection/object/P_SL-5261-167</t>
+  </si>
+  <si>
+    <t>https://media.britishmuseum.org/media/Repository/Documents/2014_9/29_18/1fcc14c8_0932_40d4_b70a_a3b50131c2a7/mid_00154511_001.jpg</t>
+  </si>
+  <si>
+    <t>https://sammlung.staedelmuseum.de/en/work/chandelier-and-coat-of-arms</t>
+  </si>
+  <si>
+    <t>Chandelier and coat of arms, ca. 1521</t>
+  </si>
+  <si>
+    <t>Albrecht Dürer: Self-Portrait with Fur-Trimmed Robe</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Albrecht_D%C3%BCrer_-_Hare,_1502_-_Google_Art_Project.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/4/44/Albrecht_D%C3%BCrer_-_Hare%2C_1502_-_Google_Art_Project.jpg</t>
+  </si>
+  <si>
+    <t>Young Hare</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Duerer_-_Ritter,_Tod_und_Teufel_(Der_Reuther).jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/8/8e/Duerer_-_Ritter%2C_Tod_und_Teufel_%28Der_Reuther%29.jpg</t>
+  </si>
+  <si>
+    <t>Knight, Death, and the Devil</t>
+  </si>
+  <si>
+    <t>m-036</t>
+  </si>
+  <si>
+    <t>m-037</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:D%C3%BCrer-Hieronymus-im-Geh%C3%A4us.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/a/ac/D%C3%BCrer-Hieronymus-im-Geh%C3%A4us.jpg</t>
+  </si>
+  <si>
+    <t>Saint Jerome in His Study</t>
+  </si>
+  <si>
+    <t>Melencolia I</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Albrecht_D%C3%BCrer_-_Melencolia_I_-_Google_Art_Project_(_AGDdr3EHmNGyA).jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/7/7a/Albrecht_D%C3%BCrer_-_Melencolia_I_-_Google_Art_Project_%28_AGDdr3EHmNGyA%29.jpg</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Albrecht-D%C3%BCrer-Haus_i_N%C3%BCrnberg_-_TEK_-_TEKA0115528.tif</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/e/e6/Albrecht-D%C3%BCrer-Haus_i_N%C3%BCrnberg_-_TEK_-_TEKA0115528.tif</t>
+  </si>
+  <si>
+    <t>m-038</t>
+  </si>
+  <si>
+    <t>m-039</t>
+  </si>
+  <si>
+    <t>m-040</t>
+  </si>
+  <si>
+    <t>m-041</t>
+  </si>
+  <si>
+    <t>m-042</t>
+  </si>
+  <si>
+    <t>m-043</t>
+  </si>
+  <si>
+    <t>m-044</t>
+  </si>
+  <si>
+    <t>m-045</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qwesPhquWsE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The video illustrates the making of an engraving, the most demanding graphic technique in Dürer's time, which Dürer introduced to Nuremberg after his journeyman travels. He created more than 100 engravings during his career. </t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/?query=search=/record/objectnumbersearch=[3063]&amp;showtype=record</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/cc/imageproxy.ashx?server=localhost&amp;port=16001&amp;filename=images/3063.JPG</t>
+  </si>
+  <si>
+    <t>Agnes Dürer ("Mein Agnes")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 year old Dürer made this intimate drawing of "His Agnes" probably shortly before their marriage in spring 1494. Agnes was then only 18 or 19 years old. With rapid pen strokes, Dürer catches this moment of drowsy thoughtfulness. Agnes will become one of Dürer's favourite models. </t>
+  </si>
+  <si>
+    <t>Kupferstich</t>
+  </si>
+  <si>
+    <t>Innsbruck von Norden</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/cc/imageproxy.ashx?server=localhost&amp;port=16001&amp;filename=images/3056.jpg</t>
+  </si>
+  <si>
+    <t>https://sammlungenonline.albertina.at/?query=search=/record/objectnumbersearch=[3056]&amp;showtype=record</t>
+  </si>
+  <si>
+    <t>This small view of Innsbruck from the North side of the Inn river is full of life. Drawn in 1496, Dürer not only portrays the cityscape on the river Inn and single buildings, but also renders ephemeral effects such as the effects of light or the reflection of houses in the water with great mastery.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 1500, 29-year-old Dürer paints himself in an unprecendented Christ-like manner. The fur coat also refers to his social status as renowned artist and well-situated citizen of Nuremberg.    </t>
+  </si>
+  <si>
+    <t>The "Young Hare", dated 1502, counts among Dürer's most famous works. The highly detailed drawing of the animal still fascinates today.</t>
+  </si>
+  <si>
+    <t>https://commons.wikimedia.org/wiki/File:Albrecht_D%C3%BCrer_-_Feast_of_Rose_Garlands_-_Google_Art_Project.jpg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/f/f9/Albrecht_D%C3%BCrer_-_Feast_of_Rose_Garlands_-_Google_Art_Project.jpg</t>
+  </si>
+  <si>
+    <t>The "Feast of the Rose Garlands" (1506) is Dürer's most Italianate painting. Among the faithful gathered around the Madonna in a "Holy Conversation", Dürer has depicted himself in the background, proudly presenting a sheet of paper with his signature. The majestic madonna, the floating garments and beautifully shaded colors, the playful putti all remind of Venetian Renaissance paintings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feast of Rose Garlands </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dürer's "Melancholia" (1514) is his best known master engraving. The winged female figure of melancholy, deep in her thoughts, is surrounded by meticulously rendered objects related to geometry, astrology and mathematics. The scribbling putto adds a playful note to this enigmatic scene which culminates in the cry of the beat-like creature. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drei Meisterstiche, Dürer's "Melancholia" (1514) is his best known master engraving. The winged female figure of melancholy, deep in her thoughts, is surrounded by meticulously rendered objects related to geometry, astrology and mathematics. The scribbling putto adds a playful note to this enigmatic scene which culminates in the cry of the beat-like creature. </t>
+  </si>
+  <si>
+    <t>Shortly after his arrival in Antwerp in August 1520, Dürer depicted this view of the harbor of the city. The quickly drawn scene is full of details and gives a lively image of the bustling atmosphere on the shores of the river Schelde.</t>
+  </si>
+  <si>
+    <t>Between 1525 and 1528, Dürer edits his three theoretical treatises, the "Theory of Perspective" (1525), the "Treatise on Fortifications" (1527), and the "Book of Proportions" (1528), published postumously by his wife Agnes. Since the beginning of the 16th century, Dürer had worked on the texts and illustrations, trying to unravel the "secrets of perspective" and different methods to calculate human proportions. Dürer's original German versions were translated into Latin and other languages.</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dürer had worked on the "Book of Proportions" for almost 25 years. It describes different methods how to calculate human proportions - male and female of different contitutions and even children. One chapter is dedicated to movements, another passage to distortions. </t>
+  </si>
+  <si>
+    <t>https://www.nuernberg.museum/img/duerer_epitaph_foto_theo-noll_2021--1-_.jpg</t>
+  </si>
+  <si>
+    <t>https://www.nuernberg.museum/projects/show/1132-albrecht-duerer-grabstaette</t>
+  </si>
+  <si>
+    <t>https://books.google.de/books?id=SpX3BoSucz0C</t>
+  </si>
+  <si>
+    <t>https://books.googleusercontent.com/books/content?req=AKW5QacMsPlzkhSCOohiXYeGljWguMgUQZpwSe9jD-AwX2dY7j4q8PfiYB4m-J-mvsYJpatZ3-Jt4fsCZCAr6gcAHgo8XQBnTUMNt41l5rsg236daxIa9HqNBkAEk1oCCB_F_p0JSetKf7xs-kEVhTq-Qbn_wXgRDnmYyENLKcPb6eOAGx0Bl8OXNIKKcW3JtNG2tTvp5CGcdn6GZGCaZWldzk6J7MFZVTFAIRyRQU9JVsHd9EG09heBzto7hdDbfN9ero7r8UITPVO7i1XxfoE6k1EHShuXtPleOELjtFzm9VrzH7cn7fY</t>
+  </si>
+  <si>
+    <t>Portrait of Agnes Dürer in a Netherlandish costume</t>
+  </si>
+  <si>
+    <t>Dürer's grave</t>
+  </si>
+  <si>
+    <t>Book of Proportions</t>
+  </si>
+  <si>
+    <t>Dürer depicted Agnes several times during their journey, among others he caught her on the ship along the Rhine valley near Boppard. In this silverpoint dawing from Dürer's sketchbook she is matched with a young girl from Cologne who probably fascinated Dürer because of her attire.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regarding the Hof van Liere, the major's residence, Dürer explicitely mentions its unsual tower, probably because of its tulip-style top which he documents in a silverpoint drawing. On the same sheet, he draws a portait of Ravensburger, a German merchant in Antwerp whom Dürer encounters severals times.  </t>
+  </si>
+  <si>
+    <t>Park of Royal Palace in Brussels: During his first stay in Brussels, Dürer had the chance to visit the royal palace. From one of the chambers on the upper floor he made this view of the vast, park-like garden of the royal residence. In the foreground, the tournament ground catches his attention.</t>
+  </si>
+  <si>
+    <t>Dürer portraits Aachen Cathedral from an upper floor window of the Town Hall. All architectonical details are clearly represented. Upon closer inspection, however, one disovers that Dürer has added one bay in the choir.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The merchant town of Bergen op Zoom is a sort of gateway to Zeeland. While waiting for his ship, Dürer has the chance to visit the town and draw some of its major monuments, among others the picturesque view of Bergen's famous Markiesenhof, the Renaissance castle of the Marquis with its characteristic "tulip" tower. </t>
+  </si>
+  <si>
+    <t>According to the inscription, Dürer depicts this head of a walrus after a real animal which was exhibited in Antwerp in 1521. It is one of his most lively animal portraits. The inscription claims that the walrus was caught "in the Netherlands sea" (e.g. the North See) and was "twelve brabant ells long with four feet”, which is more than 8 metres. Actually, walruses are only around 3.5 metres long.</t>
+  </si>
+  <si>
+    <t>Dürer depicted the two female figures in festive attire on different occasions. The left figure, very elegantly dressed in a somptous court robe and expanding headdress and full of live, was actually copied from a a brass statuette on the tomb of Isabella of Bourbon (d. 1465) in St Michael in Antwerp. The right woman, with a long mantle and characteristic hat, wears a typical attire of certain parts of Central Europe, i.e. Silesia or Eastern Austria, whom Dürer might have encountered in the trading town Antwerp or during the buzzling coronation festivities of Charles V. in Aachen and drawn in silverpoint technique.</t>
+  </si>
+  <si>
+    <t>Lucas van Leyden is a famous painter and graphic artist. He visits Dürer for a day  in spring 1521.</t>
+  </si>
+  <si>
+    <t>Portrait of a man (formerly Joachim Patinir)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dürer's grave is an iconic site since the 16th century. In the 17th century, the painter and founder of the Nuremberg art academy, Joachim von Sandrart, donated a bronze plate in veneration of his hero, and other artists strove to be buried next to Dürer in the Frey family's gravesite. </t>
+  </si>
+  <si>
+    <t>Dürer stirbt in Nürnberg und wird auf dem Johannisfriedhof begraben; Dürer died on April 6, 1528 at the age of 56 in his house in Nuremberg after a short illness. He was buried in the family grave of his parents-in-law on St John's graveyard in Nuremberg. His wife Agnes continued to run the workshop until her own death in 1539. Unlike most artists of his time, Dürer was never forgotten by posterity - on the contrary. Thanks to his outstanding art and self-promotion, his glory remains up until today.</t>
+  </si>
+  <si>
+    <t>Christian II of Denmark, who is married to Charles' V sister and stays at the court of Brussels, commissions Dürer to paint his portrait. The painting is lost, but a drawing gives an impression of Dürer's work.</t>
+  </si>
+  <si>
+    <t>Rheinfels Castle is among the most prominent medieval castles on the Rhine river. Dürer probably made this detailed view of the castle on his high hill during a travel stop or overnight stay.</t>
+  </si>
+  <si>
+    <t>https://nbn-resolving.org/urn:nbn:de:bvb:22-dtl-0000001897</t>
+  </si>
+  <si>
+    <t>Tagebuch der niederländischen Reise in einer Abschrift</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4254,17 +4839,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -4279,7 +4853,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4289,6 +4863,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4304,9 +4884,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4353,16 +4933,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4371,7 +4945,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4690,8 +5269,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4736,7 +5315,9 @@
       <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5"/>
+      <c r="J1" s="5" t="s">
+        <v>1408</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" s="10" t="s">
@@ -4747,14 +5328,21 @@
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>1386</v>
+      </c>
       <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="G2" s="10" t="s">
+        <v>1422</v>
+      </c>
       <c r="H2" s="10" t="s">
         <v>214</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>194</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>1407</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.5">
@@ -4766,7 +5354,9 @@
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>1392</v>
+      </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10" t="s">
@@ -4783,7 +5373,9 @@
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>1391</v>
+      </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10" t="s">
@@ -4800,7 +5392,9 @@
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>1393</v>
+      </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10" t="s">
@@ -4819,13 +5413,20 @@
         <v>120</v>
       </c>
       <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>1387</v>
+      </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>1415</v>
+      </c>
       <c r="H6" s="10" t="s">
         <v>215</v>
       </c>
       <c r="I6" s="10"/>
+      <c r="J6" t="s">
+        <v>1409</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A7" s="10" t="s">
@@ -4857,7 +5458,9 @@
         <v>830</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>1385</v>
+      </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10" t="s">
@@ -4891,7 +5494,9 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>1384</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="10" t="s">
@@ -4908,7 +5513,9 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="10" t="s">
+        <v>1390</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="10" t="s">
@@ -4925,7 +5532,9 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="10" t="s">
+        <v>1388</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="10" t="s">
@@ -4942,9 +5551,13 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="10" t="s">
+        <v>1389</v>
+      </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>1479</v>
+      </c>
       <c r="H13" s="10" t="s">
         <v>214</v>
       </c>
@@ -4959,40 +5572,73 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F870BEB-B6B1-493D-AF20-4CA3C7300BD9}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="86.76171875" customWidth="1"/>
+    <col min="2" max="2" width="20.1171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88" customWidth="1"/>
+    <col min="4" max="4" width="43.17578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="71.7" x14ac:dyDescent="0.5">
-      <c r="A2" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="229.35" x14ac:dyDescent="0.5">
+      <c r="A2" s="26" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="71.7" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B3" t="s">
+        <v>832</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C18" t="s">
         <v>1381</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.5">
-      <c r="B18" t="s">
-        <v>1383</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{443A0509-4DC0-4AD2-8598-6ADC36DEC702}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{B8411DE4-2CD3-4DD6-A0C5-B17E929AD716}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -5001,8 +5647,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:XFD52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -5074,7 +5720,9 @@
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="G3" s="3" t="s">
+        <v>1425</v>
+      </c>
       <c r="H3" s="10" t="s">
         <v>186</v>
       </c>
@@ -5089,8 +5737,12 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="F4" s="10" t="s">
+        <v>1547</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>1484</v>
+      </c>
       <c r="H4" s="10" t="s">
         <v>186</v>
       </c>
@@ -5108,7 +5760,9 @@
       <c r="F5" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="3" t="s">
+        <v>1485</v>
+      </c>
       <c r="H5" s="10" t="s">
         <v>192</v>
       </c>
@@ -5126,7 +5780,9 @@
       <c r="F6" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>1516</v>
+      </c>
       <c r="H6" s="10" t="s">
         <v>192</v>
       </c>
@@ -5142,9 +5798,11 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="G7" s="10"/>
+        <v>1553</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>1517</v>
+      </c>
       <c r="H7" s="10" t="s">
         <v>192</v>
       </c>
@@ -5160,7 +5818,9 @@
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>1526</v>
+      </c>
       <c r="H8" s="10" t="s">
         <v>187</v>
       </c>
@@ -5177,8 +5837,12 @@
         <v>170</v>
       </c>
       <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="F9" s="10" t="s">
+        <v>1555</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>1531</v>
+      </c>
       <c r="H9" s="10" t="s">
         <v>221</v>
       </c>
@@ -5215,19 +5879,20 @@
         <v>191</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:8" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
         <v>193</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10" t="s">
+      <c r="F12" t="s">
+        <v>1576</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>1479</v>
+      </c>
+      <c r="H12" t="s">
         <v>186</v>
       </c>
     </row>
@@ -5259,7 +5924,7 @@
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="3" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="H14" s="8" t="s">
         <v>638</v>
@@ -5275,8 +5940,12 @@
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="F15" s="10" t="s">
+        <v>1566</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>1396</v>
+      </c>
       <c r="H15" s="8" t="s">
         <v>639</v>
       </c>
@@ -5291,8 +5960,12 @@
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
+      <c r="F16" s="10" t="s">
+        <v>1566</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>1396</v>
+      </c>
       <c r="H16" s="8" t="s">
         <v>639</v>
       </c>
@@ -5308,7 +5981,9 @@
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="G17" s="10" t="s">
+        <v>1400</v>
+      </c>
       <c r="H17" s="8" t="s">
         <v>638</v>
       </c>
@@ -5324,7 +5999,9 @@
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
+      <c r="G18" s="10" t="s">
+        <v>1403</v>
+      </c>
       <c r="H18" s="8" t="s">
         <v>638</v>
       </c>
@@ -5336,11 +6013,15 @@
       <c r="B19" s="10" t="s">
         <v>488</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="10" t="s">
+        <v>1442</v>
+      </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
+      <c r="G19" s="10" t="s">
+        <v>1425</v>
+      </c>
       <c r="H19" s="8" t="s">
         <v>638</v>
       </c>
@@ -5356,7 +6037,9 @@
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
+      <c r="G20" s="10" t="s">
+        <v>1424</v>
+      </c>
       <c r="H20" s="8" t="s">
         <v>638</v>
       </c>
@@ -5388,7 +6071,9 @@
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
+      <c r="G22" s="10" t="s">
+        <v>1426</v>
+      </c>
       <c r="H22" s="8" t="s">
         <v>639</v>
       </c>
@@ -5403,8 +6088,12 @@
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
+      <c r="F23" s="10" t="s">
+        <v>1568</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>1427</v>
+      </c>
       <c r="H23" s="8" t="s">
         <v>639</v>
       </c>
@@ -5483,8 +6172,12 @@
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
+      <c r="F28" s="10" t="s">
+        <v>1565</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>1428</v>
+      </c>
       <c r="H28" s="8" t="s">
         <v>639</v>
       </c>
@@ -5499,8 +6192,12 @@
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="F29" s="10" t="s">
+        <v>1565</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>1428</v>
+      </c>
       <c r="H29" s="8" t="s">
         <v>639</v>
       </c>
@@ -5515,8 +6212,12 @@
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
+      <c r="F30" s="10" t="s">
+        <v>1569</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>1429</v>
+      </c>
       <c r="H30" s="8" t="s">
         <v>639</v>
       </c>
@@ -5532,7 +6233,9 @@
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
+      <c r="G31" s="10" t="s">
+        <v>1430</v>
+      </c>
       <c r="H31" s="8" t="s">
         <v>639</v>
       </c>
@@ -5564,7 +6267,9 @@
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
+      <c r="G33" s="10" t="s">
+        <v>1431</v>
+      </c>
       <c r="H33" s="8" t="s">
         <v>639</v>
       </c>
@@ -5596,7 +6301,9 @@
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
+      <c r="G35" s="10" t="s">
+        <v>1432</v>
+      </c>
       <c r="H35" s="8" t="s">
         <v>639</v>
       </c>
@@ -5612,7 +6319,9 @@
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
+      <c r="G36" s="10" t="s">
+        <v>1433</v>
+      </c>
       <c r="H36" s="8" t="s">
         <v>639</v>
       </c>
@@ -5675,8 +6384,12 @@
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
+      <c r="F40" s="10" t="s">
+        <v>1571</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>1423</v>
+      </c>
       <c r="H40" s="8" t="s">
         <v>639</v>
       </c>
@@ -5692,7 +6405,9 @@
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
+      <c r="G41" s="10" t="s">
+        <v>1434</v>
+      </c>
       <c r="H41" s="8" t="s">
         <v>639</v>
       </c>
@@ -5804,7 +6519,9 @@
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
+      <c r="G48" s="10" t="s">
+        <v>1435</v>
+      </c>
       <c r="H48" s="8" t="s">
         <v>639</v>
       </c>
@@ -5835,8 +6552,12 @@
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
+      <c r="F50" s="10" t="s">
+        <v>1577</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>1436</v>
+      </c>
       <c r="H50" s="8" t="s">
         <v>639</v>
       </c>
@@ -5852,7 +6573,9 @@
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
-      <c r="G51" s="10"/>
+      <c r="G51" s="10" t="s">
+        <v>1436</v>
+      </c>
       <c r="H51" s="8" t="s">
         <v>639</v>
       </c>
@@ -5868,7 +6591,9 @@
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
+      <c r="G52" s="10" t="s">
+        <v>1437</v>
+      </c>
       <c r="H52" s="8" t="s">
         <v>639</v>
       </c>
@@ -5884,7 +6609,9 @@
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
+      <c r="G53" s="10" t="s">
+        <v>1437</v>
+      </c>
       <c r="H53" s="8" t="s">
         <v>639</v>
       </c>
@@ -5932,7 +6659,9 @@
       <c r="D56" s="10"/>
       <c r="E56" s="10"/>
       <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
+      <c r="G56" s="3" t="s">
+        <v>1438</v>
+      </c>
       <c r="H56" s="8" t="s">
         <v>640</v>
       </c>
@@ -5948,7 +6677,9 @@
       <c r="D57" s="10"/>
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
+      <c r="G57" s="3" t="s">
+        <v>1439</v>
+      </c>
       <c r="H57" s="8" t="s">
         <v>640</v>
       </c>
@@ -5964,7 +6695,9 @@
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
+      <c r="G58" s="3" t="s">
+        <v>1443</v>
+      </c>
       <c r="H58" s="8" t="s">
         <v>640</v>
       </c>
@@ -5980,7 +6713,9 @@
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
+      <c r="G59" s="3" t="s">
+        <v>1444</v>
+      </c>
       <c r="H59" s="8" t="s">
         <v>640</v>
       </c>
@@ -5996,7 +6731,9 @@
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
+      <c r="G60" s="3" t="s">
+        <v>1445</v>
+      </c>
       <c r="H60" s="8" t="s">
         <v>638</v>
       </c>
@@ -6012,7 +6749,9 @@
       <c r="D61" s="10"/>
       <c r="E61" s="10"/>
       <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
+      <c r="G61" s="3" t="s">
+        <v>1446</v>
+      </c>
       <c r="H61" s="8" t="s">
         <v>638</v>
       </c>
@@ -6156,7 +6895,9 @@
       <c r="D70" s="10"/>
       <c r="E70" s="10"/>
       <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
+      <c r="G70" s="10" t="s">
+        <v>1478</v>
+      </c>
       <c r="H70" s="8" t="s">
         <v>641</v>
       </c>
@@ -6182,7 +6923,7 @@
         <v>617</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>538</v>
+        <v>1573</v>
       </c>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
@@ -6230,7 +6971,7 @@
         <v>620</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>540</v>
+        <v>1562</v>
       </c>
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
@@ -6245,14 +6986,18 @@
       <c r="A76" s="8" t="s">
         <v>621</v>
       </c>
-      <c r="B76" s="10" t="s">
+      <c r="B76" t="s">
         <v>541</v>
       </c>
       <c r="C76" s="10"/>
       <c r="D76" s="10"/>
       <c r="E76" s="10"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
+      <c r="F76" s="10" t="s">
+        <v>1576</v>
+      </c>
+      <c r="G76" s="10" t="s">
+        <v>1479</v>
+      </c>
       <c r="H76" s="8" t="s">
         <v>641</v>
       </c>
@@ -6267,8 +7012,12 @@
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
       <c r="E77" s="10"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="10"/>
+      <c r="F77" s="10" t="s">
+        <v>1572</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>1478</v>
+      </c>
       <c r="H77" s="8" t="s">
         <v>639</v>
       </c>
@@ -6316,7 +7065,9 @@
       <c r="D80" s="10"/>
       <c r="E80" s="10"/>
       <c r="F80" s="10"/>
-      <c r="G80" s="10"/>
+      <c r="G80" s="10" t="s">
+        <v>1480</v>
+      </c>
       <c r="H80" s="8" t="s">
         <v>638</v>
       </c>
@@ -6347,8 +7098,12 @@
       <c r="C82" s="10"/>
       <c r="D82" s="10"/>
       <c r="E82" s="10"/>
-      <c r="F82" s="10"/>
-      <c r="G82" s="10"/>
+      <c r="F82" s="10" t="s">
+        <v>1554</v>
+      </c>
+      <c r="G82" s="10" t="s">
+        <v>1481</v>
+      </c>
       <c r="H82" s="8" t="s">
         <v>638</v>
       </c>
@@ -6363,7 +7118,9 @@
       <c r="C83" s="10"/>
       <c r="D83" s="10"/>
       <c r="E83" s="10"/>
-      <c r="F83" s="10"/>
+      <c r="F83" s="10" t="s">
+        <v>1567</v>
+      </c>
       <c r="G83" s="10"/>
       <c r="H83" s="8" t="s">
         <v>638</v>
@@ -6379,8 +7136,12 @@
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
       <c r="E84" s="10"/>
-      <c r="F84" s="10"/>
-      <c r="G84" s="10"/>
+      <c r="F84" s="10" t="s">
+        <v>1570</v>
+      </c>
+      <c r="G84" s="10" t="s">
+        <v>1482</v>
+      </c>
       <c r="H84" s="8" t="s">
         <v>644</v>
       </c>
@@ -6525,8 +7286,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -6569,10 +7330,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>217</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>218</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -6586,10 +7347,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>697</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" t="s">
         <v>137</v>
       </c>
       <c r="H3" s="3" t="s">
@@ -6597,10 +7358,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
         <v>698</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" t="s">
         <v>648</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -6608,138 +7369,138 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>699</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A6" s="3" t="s">
+      <c r="A6" t="s">
         <v>700</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>701</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A8" s="3" t="s">
+      <c r="A8" t="s">
         <v>702</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A9" s="3" t="s">
+      <c r="A9" t="s">
         <v>703</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A10" s="3" t="s">
+      <c r="A10" t="s">
         <v>704</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>705</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" t="s">
         <v>655</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>706</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" t="s">
         <v>656</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A13" s="3" t="s">
+      <c r="A13" t="s">
         <v>707</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A14" s="3" t="s">
+      <c r="A14" t="s">
         <v>708</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A15" s="3" t="s">
+      <c r="A15" t="s">
         <v>709</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" t="s">
         <v>659</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A16" s="3" t="s">
+      <c r="A16" t="s">
         <v>710</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" t="s">
         <v>660</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A17" s="3" t="s">
+      <c r="A17" t="s">
         <v>711</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" t="s">
         <v>661</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A18" s="3" t="s">
+      <c r="A18" t="s">
         <v>712</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
         <v>713</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" t="s">
         <v>663</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>714</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A21" s="3" t="s">
+      <c r="A21" t="s">
         <v>881</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>882</v>
       </c>
       <c r="H21" s="3" t="s">
@@ -6821,7 +7582,7 @@
   <dimension ref="A1:J144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -9303,58 +10064,928 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F68774-646B-48EE-BDB5-8C878EF20F5A}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="8.9375" style="3"/>
-    <col min="2" max="2" width="28" style="3" customWidth="1"/>
-    <col min="3" max="3" width="60" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.52734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.76171875" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.9375" style="3"/>
+    <col min="2" max="2" width="38.29296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="64.703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="57.9375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.52734375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.76171875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.9375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>1382</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>1385</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>1384</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>186</v>
+      <c r="D2" s="28" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A3" s="3" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>1395</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>1394</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A5" s="3" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A6" s="3" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>1416</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A7" s="3" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>1421</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A8" s="3" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B8" t="s">
+        <v>488</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>1441</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A9" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B9" t="s">
+        <v>489</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>1448</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A10" s="3" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B10" t="s">
+        <v>491</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>1449</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A11" s="3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B11" t="s">
+        <v>492</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1451</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>1452</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A12" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>1453</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>1454</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A13" s="3" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B13" t="s">
+        <v>433</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>1457</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A14" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B14" t="s">
+        <v>499</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>1458</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A15" s="3" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B15" t="s">
+        <v>501</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>1461</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A16" s="3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B16" t="s">
+        <v>503</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A17" s="3" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B17" t="s">
+        <v>504</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>1465</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A18" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B18" t="s">
+        <v>508</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>1466</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>1467</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A19" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B19" t="s">
+        <v>509</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>1468</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>1469</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A20" s="3" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B20" t="s">
+        <v>516</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>1471</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A21" s="3" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>1473</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>1475</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A22" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1477</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>1476</v>
+      </c>
+      <c r="D22" s="30"/>
+      <c r="E22" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A23" s="3" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B23" t="s">
+        <v>524</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>1486</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>1487</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A24" s="3" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B24" t="s">
+        <v>525</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>1487</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>1488</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A25" s="3" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B25" t="s">
+        <v>526</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>1489</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>1490</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A26" s="3" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B26" t="s">
+        <v>527</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>1491</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>1492</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A27" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B27" t="s">
+        <v>528</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>1493</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A28" s="3" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B28" t="s">
+        <v>529</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>1494</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A29" s="3" t="s">
+        <v>1478</v>
+      </c>
+      <c r="B29" t="s">
+        <v>536</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>1496</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>1497</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A30" s="3" t="s">
+        <v>1479</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>1498</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>1500</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A31" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B31" t="s">
+        <v>545</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>1501</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A32" s="3" t="s">
+        <v>1481</v>
+      </c>
+      <c r="B32" t="s">
+        <v>547</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>1503</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>1504</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A33" s="3" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B33" t="s">
+        <v>549</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>1506</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A34" s="3" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1508</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>1507</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A35" s="3" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>1510</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>1511</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A36" s="3" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>1514</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A37" s="3" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>1518</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>1519</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A38" s="3" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>1523</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A39" s="3" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>1524</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>1525</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A40" s="3" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>1535</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>1535</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>1534</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A41" s="3" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>1537</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>1538</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A42" s="3" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A43" s="3" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>1551</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>1549</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A44" s="3" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>1564</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>1560</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>1561</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>1556</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A45" s="3" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>1559</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>1558</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A46" s="3" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>1578</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>1556</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{6555C001-AF61-499A-ABE7-287E901E3F73}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{6555C001-AF61-499A-ABE7-287E901E3F73}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{3A277AAE-8FCE-499A-AE78-309DEB57D14E}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{FF537007-C8B6-422B-B764-A977081C356D}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{01803DF9-95A9-4673-B3CF-0AFDC51738A6}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{2035CEB9-3894-4D0E-A800-0EDCBF47DCB0}"/>
+    <hyperlink ref="C5" r:id="rId6" xr:uid="{0A79A952-20B9-42A0-96C2-1DF0D3009FCE}"/>
+    <hyperlink ref="C4" r:id="rId7" xr:uid="{C448F71C-0442-4884-8E94-74AB850D546C}"/>
+    <hyperlink ref="D6" r:id="rId8" xr:uid="{7D5EB142-335B-4476-B272-FD9F53933C39}"/>
+    <hyperlink ref="C6" r:id="rId9" xr:uid="{CCDBF689-403E-43A8-BED9-3E755171E066}"/>
+    <hyperlink ref="C7" r:id="rId10" xr:uid="{64183D9C-D3CF-4202-B5C3-18F54B30105D}"/>
+    <hyperlink ref="D8" r:id="rId11" display="https://www.bildindex.de/media/large/mi/03/97/6a/mi03976a05.jpg?Expires=1677759882&amp;Signature=hWeVgz5cjlYCBB2LCiBgpEX8KcG3RfTFq0uPL84nDEqrdHhy5ubRwrJVjKuEWzf92X13ypwWFMGToksoUmCw2HPJSF~1JI8zBmob43tSWRXG7P0H5U3DKehqf2tfXUma7o~ZU42ct2Rf9FcwuOsC6EEw2QvAlzU7pO6W7wfrA18_&amp;Key-Pair-Id=APKAJGHHKKX2FHRP63AQ" xr:uid="{2BDCDC4C-CAC4-44B7-B28C-83BD8753952C}"/>
+    <hyperlink ref="C8" r:id="rId12" xr:uid="{63355708-FBD7-4D22-AECF-34AD1D7C138F}"/>
+    <hyperlink ref="C9" r:id="rId13" xr:uid="{480D5B27-8454-41B3-A50B-4ACFFDAE4026}"/>
+    <hyperlink ref="D9" r:id="rId14" xr:uid="{1E9B9CA0-D6F1-4AE0-AE43-7776F5BD6EF1}"/>
+    <hyperlink ref="D10" r:id="rId15" xr:uid="{EA214F1E-4812-477F-90AE-31C9F30296F1}"/>
+    <hyperlink ref="C10" r:id="rId16" xr:uid="{9FE6D3D1-53E9-489A-AB96-5EC7DADDD591}"/>
+    <hyperlink ref="D11" r:id="rId17" xr:uid="{B87A9B74-3BD6-4ED9-98AB-34EDAE07337F}"/>
+    <hyperlink ref="C12" r:id="rId18" xr:uid="{5D03CC0B-DEE3-4FDE-9306-CE5E26709C32}"/>
+    <hyperlink ref="C13" r:id="rId19" xr:uid="{FFAAC713-605F-4948-894C-B32F62D6C8E4}"/>
+    <hyperlink ref="D13" r:id="rId20" xr:uid="{A0893C3E-1C28-467D-9AFC-E8EE4AB9FB89}"/>
+    <hyperlink ref="D14" r:id="rId21" xr:uid="{3F64321A-2515-493E-917E-72B791B9408D}"/>
+    <hyperlink ref="C14" r:id="rId22" xr:uid="{0332E7E1-BC6A-47EA-89D6-97A7068AB01F}"/>
+    <hyperlink ref="C15" r:id="rId23" xr:uid="{6EC68279-7666-4082-ADEA-A2C7658064D2}"/>
+    <hyperlink ref="D16" r:id="rId24" xr:uid="{517CD509-8487-4373-A454-B2B9E47FF545}"/>
+    <hyperlink ref="C16" r:id="rId25" xr:uid="{29844E65-FF0E-4D48-82B8-096506F811E6}"/>
+    <hyperlink ref="C17" r:id="rId26" xr:uid="{28A376E3-CC6D-491B-96A1-EB17AA4EFB22}"/>
+    <hyperlink ref="C18" r:id="rId27" xr:uid="{412FF679-225E-44C0-8E9F-CFBE4329EBC3}"/>
+    <hyperlink ref="D18" r:id="rId28" xr:uid="{F8DEBD7A-3831-43DB-A095-2BC3CECE35C2}"/>
+    <hyperlink ref="C19" r:id="rId29" xr:uid="{7C9CB129-6FFC-4285-AC98-069E1A3CCCC6}"/>
+    <hyperlink ref="D19" r:id="rId30" xr:uid="{CE60D295-56DA-4DAD-ABF8-FA73AB5B855E}"/>
+    <hyperlink ref="C20" r:id="rId31" xr:uid="{234F6491-E60B-4B87-A632-870076D9CCA7}"/>
+    <hyperlink ref="C21" r:id="rId32" xr:uid="{61D9836A-7C7E-4867-ABF5-33BB8C69892E}"/>
+    <hyperlink ref="D21" r:id="rId33" xr:uid="{ABE00576-9886-4B0A-A870-5D91CF571100}"/>
+    <hyperlink ref="C22" r:id="rId34" xr:uid="{D4605030-C409-4AF3-8259-809032BBDE3E}"/>
+    <hyperlink ref="C25" r:id="rId35" xr:uid="{080340CC-9D67-448D-91B8-CF5E61F24528}"/>
+    <hyperlink ref="C26" r:id="rId36" xr:uid="{2C13BE1F-6959-4279-B9CC-BE2550EA0D05}"/>
+    <hyperlink ref="C27" r:id="rId37" xr:uid="{161A5A2E-4114-4985-9828-82028E172B03}"/>
+    <hyperlink ref="D28" r:id="rId38" xr:uid="{C7E1F470-0BA6-453D-B307-2A7B184F5CBB}"/>
+    <hyperlink ref="C28" r:id="rId39" xr:uid="{11E684AC-C433-4034-B87F-E540C77A524F}"/>
+    <hyperlink ref="C29" r:id="rId40" xr:uid="{6B023398-4DAE-4F93-81D4-CF7601909568}"/>
+    <hyperlink ref="C30" r:id="rId41" xr:uid="{0C9432DA-F217-44DE-B2FF-70283A13F215}"/>
+    <hyperlink ref="D30" r:id="rId42" xr:uid="{5AFC87AF-12FB-4162-8E98-DF8E161DC898}"/>
+    <hyperlink ref="D31" r:id="rId43" xr:uid="{55865B39-4DCB-4D60-B607-52D2D3ADFF82}"/>
+    <hyperlink ref="C31" r:id="rId44" xr:uid="{B70145B5-B167-4A5B-8D5E-B5EBC65F3C2B}"/>
+    <hyperlink ref="C32" r:id="rId45" xr:uid="{ED6D5FE2-EE49-483E-B19B-37602DF833A2}"/>
+    <hyperlink ref="D7" r:id="rId46" xr:uid="{F5CD6900-3559-4D8F-8717-FF92BEE78CF8}"/>
+    <hyperlink ref="C35" r:id="rId47" xr:uid="{DBA5A372-746C-4C4C-815B-81F869194C86}"/>
+    <hyperlink ref="D35" r:id="rId48" xr:uid="{4D09EA8C-4FA5-43D4-83C6-8F98113BD100}"/>
+    <hyperlink ref="C36" r:id="rId49" xr:uid="{FEDE9C89-95F5-405A-B824-83ACDC1592FF}"/>
+    <hyperlink ref="C37" r:id="rId50" xr:uid="{8E39BE0E-9C8D-4504-94B0-4A6D54597337}"/>
+    <hyperlink ref="D37" r:id="rId51" xr:uid="{4F366ACA-E9DC-4D82-A164-F3C23305A963}"/>
+    <hyperlink ref="C38" r:id="rId52" xr:uid="{1ED5BD43-7A12-48C2-BC69-8F0EBCC5B3A0}"/>
+    <hyperlink ref="D38" r:id="rId53" xr:uid="{F2EA09DA-74A9-46C8-AF66-8E4B1AB4C1B9}"/>
+    <hyperlink ref="C39" r:id="rId54" xr:uid="{049280BA-CFC9-44A0-A076-2331B0E40C26}"/>
+    <hyperlink ref="C40" r:id="rId55" xr:uid="{9C52C1E3-7BD1-4B41-A23E-81A351F47D54}"/>
+    <hyperlink ref="D40" r:id="rId56" xr:uid="{EC6045AC-7661-4396-876E-A185378B4D91}"/>
+    <hyperlink ref="C41" r:id="rId57" xr:uid="{D1BD7645-D58F-40F7-978F-383E3AB8995C}"/>
+    <hyperlink ref="D42" r:id="rId58" xr:uid="{6DA96B2C-01E1-4702-8D73-C6CB924302ED}"/>
+    <hyperlink ref="C42" r:id="rId59" xr:uid="{70FE4ABE-035F-4403-A099-051396E69EF1}"/>
+    <hyperlink ref="C43" r:id="rId60" xr:uid="{A6B885F7-852B-4C3F-896A-81B7A4085B52}"/>
+    <hyperlink ref="D45" r:id="rId61" xr:uid="{2AFA1DCA-150C-4E59-B51B-408C4EE4D9F1}"/>
+    <hyperlink ref="C45" r:id="rId62" xr:uid="{7C291294-21B9-4C11-8570-25513F54FB58}"/>
+    <hyperlink ref="C44" r:id="rId63" xr:uid="{CBEA5E2B-AF57-44B8-A639-1B5A04764DA8}"/>
+    <hyperlink ref="D44" r:id="rId64" display="https://books.googleusercontent.com/books/content?req=AKW5QacMsPlzkhSCOohiXYeGljWguMgUQZpwSe9jD-AwX2dY7j4q8PfiYB4m-J-mvsYJpatZ3-Jt4fsCZCAr6gcAHgo8XQBnTUMNt41l5rsg236daxIa9HqNBkAEk1oCCB_F_p0JSetKf7xs-kEVhTq-Qbn_wXgRDnmYyENLKcPb6eOAGx0Bl8OXNIKKcW3JtNG2tTvp5CGcdn6GZGCaZWldzk6J7MFZVTFAIRyRQU9JVsHd9EG09heBzto7hdDbfN9ero7r8UITPVO7i1XxfoE6k1EHShuXtPleOELjtFzm9VrzH7cn7fY" xr:uid="{90E85313-5E40-414D-9C42-229BB197B0DE}"/>
+    <hyperlink ref="C46" r:id="rId65" xr:uid="{F2BAF4A6-985D-44AC-9ECB-2096E65D0F5C}"/>
+    <hyperlink ref="D46" r:id="rId66" xr:uid="{E6F296C4-41E7-4352-9AA6-816879210698}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId67"/>
 </worksheet>
 </file>
 
@@ -9363,8 +10994,8 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:N241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -13753,8 +15384,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -13833,7 +15464,7 @@
       <c r="D2" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="24" t="s">
         <v>87</v>
       </c>
       <c r="F2" s="11" t="s">
@@ -13867,7 +15498,7 @@
       <c r="D3" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="26"/>
+      <c r="E3" s="24"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -14091,7 +15722,7 @@
       <c r="D11" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="24" t="s">
         <v>125</v>
       </c>
       <c r="F11" s="11" t="s">
@@ -14227,7 +15858,7 @@
       <c r="D15" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="24" t="s">
         <v>127</v>
       </c>
       <c r="F15" s="11" t="s">
@@ -14259,7 +15890,7 @@
       <c r="D16" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="26"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="12"/>
@@ -14475,7 +16106,7 @@
       <c r="D24" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="24" t="s">
         <v>148</v>
       </c>
       <c r="F24" s="11" t="s">
@@ -14509,7 +16140,7 @@
       <c r="D25" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="24" t="s">
         <v>148</v>
       </c>
       <c r="F25" s="11" t="s">
@@ -14543,7 +16174,7 @@
       <c r="D26" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="24" t="s">
         <v>148</v>
       </c>
       <c r="F26" s="11" t="s">
@@ -14911,7 +16542,7 @@
       <c r="D39" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="26" t="s">
+      <c r="E39" s="24" t="s">
         <v>220</v>
       </c>
       <c r="F39" s="11" t="s">
@@ -15664,7 +17295,7 @@
         <v>99</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>173</v>
+        <v>1575</v>
       </c>
       <c r="F64" s="11" t="s">
         <v>172</v>
@@ -15695,8 +17326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DE7CD6-3992-47BC-A701-56D724BB2518}">
   <dimension ref="A1:N169"/>
   <sheetViews>
-    <sheetView topLeftCell="E118" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127:XFD127"/>
+    <sheetView topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -15708,46 +17339,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.5">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="25" t="s">
         <v>836</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="25" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added media and biography import
</commit_message>
<xml_diff>
--- a/public/data/data-duerer.xlsx
+++ b/public/data/data-duerer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\duk\InTaVia2023\data-import\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFC628D-7D5A-4CD7-A34B-DF1CA718B97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174BC348-ABBC-4795-B895-0B62602C4357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" xr2:uid="{C25329CA-05B7-420C-A3AD-7BFC7999E524}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" firstSheet="1" activeTab="9" xr2:uid="{C25329CA-05B7-420C-A3AD-7BFC7999E524}"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4119" uniqueCount="1580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4116" uniqueCount="1581">
   <si>
     <t>id</t>
   </si>
@@ -4213,9 +4213,6 @@
   </si>
   <si>
     <t>gnd:119195380</t>
-  </si>
-  <si>
-    <t>wiki:Q1990389</t>
   </si>
   <si>
     <t>gnd:118771175</t>
@@ -4786,6 +4783,12 @@
   </si>
   <si>
     <t>Tagebuch der niederländischen Reise in einer Abschrift</t>
+  </si>
+  <si>
+    <t>q:Q1990389</t>
+  </si>
+  <si>
+    <t>citation</t>
   </si>
 </sst>
 </file>
@@ -5269,8 +5272,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -5316,7 +5319,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.5">
@@ -5333,7 +5336,7 @@
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>214</v>
@@ -5342,7 +5345,7 @@
         <v>194</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.5">
@@ -5355,7 +5358,7 @@
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
@@ -5374,7 +5377,7 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -5393,7 +5396,7 @@
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -5418,14 +5421,14 @@
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>215</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.5">
@@ -5514,7 +5517,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="10" t="s">
-        <v>1390</v>
+        <v>1579</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -5556,7 +5559,7 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>214</v>
@@ -5572,70 +5575,60 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F870BEB-B6B1-493D-AF20-4CA3C7300BD9}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="20.1171875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88" customWidth="1"/>
-    <col min="4" max="4" width="43.17578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88" customWidth="1"/>
+    <col min="3" max="3" width="43.17578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>1409</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="229.35" x14ac:dyDescent="0.5">
+      <c r="A2" s="26" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>1410</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="229.35" x14ac:dyDescent="0.5">
-      <c r="A2" s="26" t="s">
-        <v>1407</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="27" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="71.7" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>1412</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>1411</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="71.7" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>1409</v>
-      </c>
-      <c r="B3" t="s">
-        <v>832</v>
-      </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>1413</v>
       </c>
-      <c r="D3" s="28" t="s">
-        <v>1414</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.5">
-      <c r="C18" t="s">
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.5">
+      <c r="B18" t="s">
         <v>1381</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{443A0509-4DC0-4AD2-8598-6ADC36DEC702}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{B8411DE4-2CD3-4DD6-A0C5-B17E929AD716}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{443A0509-4DC0-4AD2-8598-6ADC36DEC702}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{B8411DE4-2CD3-4DD6-A0C5-B17E929AD716}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -5648,7 +5641,7 @@
   <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -5721,7 +5714,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="3" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>186</v>
@@ -5738,10 +5731,10 @@
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>186</v>
@@ -5761,7 +5754,7 @@
         <v>162</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>192</v>
@@ -5781,7 +5774,7 @@
         <v>162</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>192</v>
@@ -5798,10 +5791,10 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>192</v>
@@ -5819,7 +5812,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>187</v>
@@ -5838,10 +5831,10 @@
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>221</v>
@@ -5887,10 +5880,10 @@
         <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="H12" t="s">
         <v>186</v>
@@ -5941,10 +5934,10 @@
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>639</v>
@@ -5961,10 +5954,10 @@
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>639</v>
@@ -5982,7 +5975,7 @@
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>638</v>
@@ -6000,7 +5993,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>638</v>
@@ -6014,13 +6007,13 @@
         <v>488</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>638</v>
@@ -6038,7 +6031,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>638</v>
@@ -6072,7 +6065,7 @@
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>639</v>
@@ -6089,10 +6082,10 @@
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>639</v>
@@ -6173,10 +6166,10 @@
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>639</v>
@@ -6193,10 +6186,10 @@
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>639</v>
@@ -6213,10 +6206,10 @@
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>639</v>
@@ -6234,7 +6227,7 @@
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="H31" s="8" t="s">
         <v>639</v>
@@ -6268,7 +6261,7 @@
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="H33" s="8" t="s">
         <v>639</v>
@@ -6302,7 +6295,7 @@
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="H35" s="8" t="s">
         <v>639</v>
@@ -6320,7 +6313,7 @@
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="H36" s="8" t="s">
         <v>639</v>
@@ -6385,10 +6378,10 @@
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="H40" s="8" t="s">
         <v>639</v>
@@ -6406,7 +6399,7 @@
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="H41" s="8" t="s">
         <v>639</v>
@@ -6520,7 +6513,7 @@
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="H48" s="8" t="s">
         <v>639</v>
@@ -6553,10 +6546,10 @@
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>639</v>
@@ -6574,7 +6567,7 @@
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
       <c r="G51" s="10" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>639</v>
@@ -6592,7 +6585,7 @@
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="H52" s="8" t="s">
         <v>639</v>
@@ -6610,7 +6603,7 @@
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>639</v>
@@ -6660,7 +6653,7 @@
       <c r="E56" s="10"/>
       <c r="F56" s="10"/>
       <c r="G56" s="3" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="H56" s="8" t="s">
         <v>640</v>
@@ -6678,7 +6671,7 @@
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
       <c r="G57" s="3" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="H57" s="8" t="s">
         <v>640</v>
@@ -6696,7 +6689,7 @@
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
       <c r="G58" s="3" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="H58" s="8" t="s">
         <v>640</v>
@@ -6714,7 +6707,7 @@
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
       <c r="G59" s="3" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="H59" s="8" t="s">
         <v>640</v>
@@ -6732,7 +6725,7 @@
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
       <c r="G60" s="3" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="H60" s="8" t="s">
         <v>638</v>
@@ -6750,7 +6743,7 @@
       <c r="E61" s="10"/>
       <c r="F61" s="10"/>
       <c r="G61" s="3" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="H61" s="8" t="s">
         <v>638</v>
@@ -6896,7 +6889,7 @@
       <c r="E70" s="10"/>
       <c r="F70" s="10"/>
       <c r="G70" s="10" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="H70" s="8" t="s">
         <v>641</v>
@@ -6923,7 +6916,7 @@
         <v>617</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
@@ -6971,7 +6964,7 @@
         <v>620</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
@@ -6993,10 +6986,10 @@
       <c r="D76" s="10"/>
       <c r="E76" s="10"/>
       <c r="F76" s="10" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="H76" s="8" t="s">
         <v>641</v>
@@ -7013,10 +7006,10 @@
       <c r="D77" s="10"/>
       <c r="E77" s="10"/>
       <c r="F77" s="10" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="H77" s="8" t="s">
         <v>639</v>
@@ -7066,7 +7059,7 @@
       <c r="E80" s="10"/>
       <c r="F80" s="10"/>
       <c r="G80" s="10" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="H80" s="8" t="s">
         <v>638</v>
@@ -7099,10 +7092,10 @@
       <c r="D82" s="10"/>
       <c r="E82" s="10"/>
       <c r="F82" s="10" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="H82" s="8" t="s">
         <v>638</v>
@@ -7119,7 +7112,7 @@
       <c r="D83" s="10"/>
       <c r="E83" s="10"/>
       <c r="F83" s="10" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="G83" s="10"/>
       <c r="H83" s="8" t="s">
@@ -7137,10 +7130,10 @@
       <c r="D84" s="10"/>
       <c r="E84" s="10"/>
       <c r="F84" s="10" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="H84" s="8" t="s">
         <v>644</v>
@@ -10066,7 +10059,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A47" sqref="A47:A53"/>
     </sheetView>
   </sheetViews>
@@ -10106,13 +10099,13 @@
         <v>1380</v>
       </c>
       <c r="B2" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>1382</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>1383</v>
@@ -10120,33 +10113,33 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B3" t="s">
         <v>1396</v>
       </c>
-      <c r="B3" t="s">
-        <v>1397</v>
-      </c>
       <c r="C3" s="28" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B4" t="s">
         <v>1400</v>
       </c>
-      <c r="B4" t="s">
-        <v>1401</v>
-      </c>
       <c r="C4" s="28" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="D4" s="30"/>
       <c r="E4" s="3" t="s">
@@ -10155,16 +10148,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B5" t="s">
         <v>1403</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="28" t="s">
         <v>1404</v>
       </c>
-      <c r="C5" s="28" t="s">
-        <v>1405</v>
-      </c>
       <c r="D5" s="28" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>1383</v>
@@ -10172,56 +10165,56 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D6" s="28" t="s">
         <v>1415</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1417</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>1418</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>1416</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F6" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="B7" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="C7" s="28" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>1420</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>1421</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="B8" t="s">
         <v>488</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>1383</v>
@@ -10229,16 +10222,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B9" t="s">
         <v>489</v>
       </c>
       <c r="C9" s="28" t="s">
+        <v>1446</v>
+      </c>
+      <c r="D9" s="28" t="s">
         <v>1447</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>1448</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>1383</v>
@@ -10246,16 +10239,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="B10" t="s">
         <v>491</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>1383</v>
@@ -10263,93 +10256,93 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="B11" t="s">
         <v>492</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D11" s="28" t="s">
         <v>1451</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>1452</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="B12" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="C12" s="28" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>1453</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>1454</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F12" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="B13" t="s">
         <v>433</v>
       </c>
       <c r="C13" s="28" t="s">
+        <v>1455</v>
+      </c>
+      <c r="D13" s="28" t="s">
         <v>1456</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>1457</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14" s="3" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="B14" t="s">
         <v>499</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15" s="3" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="B15" t="s">
         <v>501</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="3" t="s">
@@ -10358,16 +10351,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16" s="3" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="B16" t="s">
         <v>503</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>1383</v>
@@ -10375,16 +10368,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" s="3" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="B17" t="s">
         <v>504</v>
       </c>
       <c r="C17" s="28" t="s">
+        <v>1463</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>1464</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>1465</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>1383</v>
@@ -10392,36 +10385,36 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="3" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="B18" t="s">
         <v>508</v>
       </c>
       <c r="C18" s="28" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D18" s="28" t="s">
         <v>1466</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>1467</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="3" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="B19" t="s">
         <v>509</v>
       </c>
       <c r="C19" s="28" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D19" s="28" t="s">
         <v>1468</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>1469</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>1383</v>
@@ -10429,16 +10422,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="3" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="B20" t="s">
         <v>516</v>
       </c>
       <c r="C20" s="28" t="s">
+        <v>1469</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>1470</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>1471</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>1383</v>
@@ -10446,33 +10439,33 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="3" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B21" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D21" s="28" t="s">
         <v>1474</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>1473</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>1475</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="3" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="B22" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="D22" s="30"/>
       <c r="E22" s="3" t="s">
@@ -10481,16 +10474,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23" s="3" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="B23" t="s">
         <v>524</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>1486</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>1487</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>1383</v>
@@ -10498,16 +10491,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24" s="3" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="B24" t="s">
         <v>525</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>1486</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>1487</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>1488</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>1383</v>
@@ -10515,16 +10508,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25" s="3" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="B25" t="s">
         <v>526</v>
       </c>
       <c r="C25" s="28" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>1489</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>1490</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>1383</v>
@@ -10532,16 +10525,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26" s="3" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B26" t="s">
         <v>527</v>
       </c>
       <c r="C26" s="28" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>1491</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>1492</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>1383</v>
@@ -10549,13 +10542,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A27" s="3" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="B27" t="s">
         <v>528</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>1383</v>
@@ -10563,16 +10556,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A28" s="3" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="B28" t="s">
         <v>529</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>1383</v>
@@ -10580,16 +10573,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29" s="3" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="B29" t="s">
         <v>536</v>
       </c>
       <c r="C29" s="28" t="s">
+        <v>1495</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>1496</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>1497</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>1383</v>
@@ -10597,36 +10590,36 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30" s="3" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="B30" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>1497</v>
+      </c>
+      <c r="D30" s="28" t="s">
         <v>1499</v>
-      </c>
-      <c r="C30" s="28" t="s">
-        <v>1498</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>1500</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A31" s="3" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="B31" t="s">
         <v>545</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>1383</v>
@@ -10634,53 +10627,53 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A32" s="3" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="B32" t="s">
         <v>547</v>
       </c>
       <c r="C32" s="28" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>1503</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>1504</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A33" s="3" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="B33" t="s">
         <v>549</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>1504</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>1505</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>1506</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A34" s="3" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="B34" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>1383</v>
@@ -10688,36 +10681,36 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A35" s="3" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="C35" s="28" t="s">
+        <v>1509</v>
+      </c>
+      <c r="D35" s="28" t="s">
         <v>1510</v>
-      </c>
-      <c r="D35" s="28" t="s">
-        <v>1511</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A36" s="3" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="C36" s="28" t="s">
+        <v>1512</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>1513</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>1514</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>1383</v>
@@ -10725,16 +10718,16 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A37" s="3" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="C37" s="28" t="s">
+        <v>1517</v>
+      </c>
+      <c r="D37" s="28" t="s">
         <v>1518</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>1519</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>1383</v>
@@ -10742,36 +10735,36 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A38" s="3" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C38" s="28" t="s">
         <v>1521</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="D38" s="31" t="s">
         <v>1522</v>
-      </c>
-      <c r="D38" s="31" t="s">
-        <v>1523</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A39" s="3" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>175</v>
       </c>
       <c r="C39" s="28" t="s">
+        <v>1523</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>1524</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>1525</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>1383</v>
@@ -10779,139 +10772,139 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A40" s="3" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="C40" s="28" t="s">
+        <v>1534</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>1534</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>1533</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>1535</v>
-      </c>
-      <c r="D40" s="28" t="s">
-        <v>1535</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>1534</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>1536</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A41" s="3" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="C41" s="28" t="s">
+        <v>1536</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>1537</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>1538</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A42" s="3" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>1543</v>
+      </c>
+      <c r="D42" s="28" t="s">
         <v>1542</v>
-      </c>
-      <c r="C42" s="28" t="s">
-        <v>1544</v>
-      </c>
-      <c r="D42" s="28" t="s">
-        <v>1543</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A43" s="3" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="C43" s="28" t="s">
+        <v>1547</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>1548</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>1549</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A44" s="3" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="C44" s="28" t="s">
+        <v>1559</v>
+      </c>
+      <c r="D44" s="28" t="s">
         <v>1560</v>
       </c>
-      <c r="D44" s="28" t="s">
-        <v>1561</v>
-      </c>
       <c r="E44" s="3" t="s">
+        <v>1555</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>1556</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>1557</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A45" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>1383</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A46" s="3" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="D46" s="28" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
   </sheetData>
@@ -17295,7 +17288,7 @@
         <v>99</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="F64" s="11" t="s">
         <v>172</v>
@@ -17326,7 +17319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DE7CD6-3992-47BC-A701-56D724BB2518}">
   <dimension ref="A1:N169"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" workbookViewId="0">
+    <sheetView topLeftCell="A89" workbookViewId="0">
       <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
case studies data and generated fixtures
</commit_message>
<xml_diff>
--- a/public/data/data-duerer.xlsx
+++ b/public/data/data-duerer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\duk\InTaVia2023\data-import\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89532730-5AD6-49CE-B340-0136D6DEDCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F901E4-AEBD-43CC-BA0A-5D8F062BF370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" firstSheet="1" activeTab="2" xr2:uid="{C25329CA-05B7-420C-A3AD-7BFC7999E524}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" tabRatio="647" firstSheet="4" activeTab="8" xr2:uid="{C25329CA-05B7-420C-A3AD-7BFC7999E524}"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="1" r:id="rId1"/>
@@ -7295,7 +7295,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -17369,14 +17369,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DE7CD6-3992-47BC-A701-56D724BB2518}">
   <dimension ref="A1:N169"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="60.17578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="100.64453125" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="3" max="3" width="13.1171875" customWidth="1"/>
+    <col min="5" max="5" width="30.64453125" customWidth="1"/>
     <col min="6" max="6" width="12.9375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.9375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>